<commit_message>
Revert "UI, 튜토리얼 수정"
This reverts commit 709abe63788067752a27f60a7074f0afdf297a8b.
</commit_message>
<xml_diff>
--- a/AlgorithmDefense/Assets/ExcelImporter/StageDataTable.xlsx
+++ b/AlgorithmDefense/Assets/ExcelImporter/StageDataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unityproject\AlgorithmDefense-main\AlgorithmDefense\Assets\ExcelImporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Unity\AlgorithmDefense\AlgorithmDefense\Assets\ExcelImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40C06A-610A-4148-AB97-3525204DA732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD09154D-3992-472F-BB0F-78C5FBA404F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1965" windowWidth="14025" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="2985" windowWidth="22890" windowHeight="11010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StageNum" sheetId="1" r:id="rId1"/>
@@ -110,15 +110,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>-1,-1,-1,-1,4,-1,-1,0,-1,3,1,-1,-1,2,-1,-1,-1,-1,-1,-1,-1,-1,-1,-1,-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>-1,-1,-1,-1,4,-1,-1,-1,-1,-1,-1,-1,0,-1,-1,1,-1,-1,-1,3,-1,0,-1,-1,-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-1,-1,-1,-1,3,-1,-1,0,-1,-1,4,-1,-1,2,-1,-1,1,-1,-1,-1,-1,-1,-1,0,-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-1,-1,-1,-1,-1,2,-1,1,-1,-1,-1,-1,-1,-1,-1,0,-1,0,-1,3,-1,4,-1,-1,-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -788,7 +788,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -818,10 +818,10 @@
         <v>21</v>
       </c>
       <c r="C2" s="14">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D2" s="14">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -832,10 +832,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="14">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1000</v>
+        <v>3000</v>
+      </c>
+      <c r="D3" s="15">
+        <v>3000</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -843,13 +843,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="14">
-        <v>1000</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -857,13 +857,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="15">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D5" s="15">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -871,13 +871,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="15">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D6" s="15">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
G-Star 2022 최종 수정안.
</commit_message>
<xml_diff>
--- a/AlgorithmDefense/Assets/ExcelImporter/StageDataTable.xlsx
+++ b/AlgorithmDefense/Assets/ExcelImporter/StageDataTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pj\Test\AlgorithmDefense\AlgorithmDefense\AlgorithmDefense\Assets\ExcelImporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unityproject\AlgorithmDefense-main\AlgorithmDefense\Assets\ExcelImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB558672-9EDF-4BB7-9817-3B56BEA7B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1965" windowWidth="14025" windowHeight="11280" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StageNum" sheetId="1" r:id="rId1"/>
@@ -21,14 +22,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -105,26 +98,26 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-1,-1,-1,-1,-1,-1,2,-1,-1,4,-1,-1,-1,1,-1,-1,-1,0,-1,-1,-1,-1,-1,-1,-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-1,-1,-1,-1,4,-1,-1,-1,-1,-1,-1,-1,0,-1,-1,1,-1,-1,-1,3,-1,0,-1,-1,-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>-1,-1,-1,-1,3,-1,-1,0,-1,-1,4,-1,-1,2,-1,-1,1,-1,-1,-1,-1,-1,-1,0,-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-1,-1,-1,-1,-1,2,-1,1,-1,-1,-1,-1,-1,-1,-1,0,-1,0,-1,3,-1,4,-1,-1,-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1,-1,-1,-1,4,-1,-1,0,-1,-1,-1,-1,-1,-1,-1,1,-1,-1,-1,3,-1,0,-1,-1,-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1,-1,-1,-1,-1,-1,2,-1,-1,4,-1,-1,0,-1,-1,-1,-1,-1,1,-1,-1,-1,-1,-1,-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -677,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -785,11 +778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -819,7 +812,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="14">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D2" s="14">
         <v>1000</v>
@@ -830,10 +823,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" s="14">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D3" s="14">
         <v>1000</v>
@@ -844,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14">
         <v>1000</v>
@@ -858,13 +851,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="15">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="D5" s="15">
-        <v>2000</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -872,13 +865,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="15">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="D6" s="15">
-        <v>2000</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" customHeight="1" thickBot="1">
@@ -911,7 +904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>